<commit_message>
update verb be - test merge excel
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="2115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14715" windowHeight="3435"/>
   </bookViews>
   <sheets>
     <sheet name="most-common-verbs-english" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4947" uniqueCount="3975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="3977">
   <si>
     <t>Word</t>
   </si>
@@ -11936,10 +11936,16 @@
     <t>classified</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>m4</t>
   </si>
 </sst>
 </file>
@@ -12781,11 +12787,11 @@
       <c r="C2" t="s">
         <v>3974</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
+      <c r="D2" t="s">
+        <v>3975</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3976</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>